<commit_message>
updated data for snps
</commit_message>
<xml_diff>
--- a/highconfidencesnps_temptrial.xlsx
+++ b/highconfidencesnps_temptrial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luyangzhang/Desktop/deaminase/deaminase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4318A8A4-0B47-4642-A84E-244C15FC170C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35989677-15C6-C543-81C0-F6662EB54EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="820" windowWidth="30240" windowHeight="17440" xr2:uid="{BFB935B0-CD33-FD4E-BEFC-7137ADEE7339}"/>
+    <workbookView xWindow="0" yWindow="820" windowWidth="20240" windowHeight="17440" xr2:uid="{BFB935B0-CD33-FD4E-BEFC-7137ADEE7339}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BAC1E73-C8C8-8347-B96C-C434D755D82E}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="O61" sqref="O61"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>